<commit_message>
solucion de envios indiviiduales
</commit_message>
<xml_diff>
--- a/public/files/sms_campaing.xlsx
+++ b/public/files/sms_campaing.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C590B351-62E0-6845-B10A-3A2CB120F42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,20 +363,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I3"/>
+      <selection activeCell="K8" sqref="A2:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,64 +403,6 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>94571290</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>94571290</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>